<commit_message>
added C45 Classifier (not working yet) refactored and renamed
</commit_message>
<xml_diff>
--- a/doc/computers.xlsx
+++ b/doc/computers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenix/Desktop/WORKSPACES/WDK.git/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F0C079-0BC2-0248-892A-02A9FFEC74F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7EA812-5736-FF4A-8361-3D9AB7E10BAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23520" yWindow="560" windowWidth="44100" windowHeight="27180" activeTab="3" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
+    <workbookView xWindow="13400" yWindow="5360" windowWidth="44100" windowHeight="27180" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="preprocessing" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="segmentation" sheetId="3" r:id="rId3"/>
     <sheet name="computers" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>HighPassFilter</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Magnitude</t>
   </si>
   <si>
-    <t>![Magnitude](https://latex.codecogs.com/gif.latex?M%28x_i%29%20%3D%20%5Csqrt%7Ba_x%28x_i%29%5E2%20&amp;plus;%20a_y%28x_i%29%5E2%20&amp;plus;%20a_z%28x_i%29%5E2%29%7D)</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -349,6 +346,15 @@
   </si>
   <si>
     <t>n/2</t>
+  </si>
+  <si>
+    <t>Butterworth Low-pass filter</t>
+  </si>
+  <si>
+    <t>å</t>
+  </si>
+  <si>
+    <t>![Magnitude](https://latex.codecogs.com/gif.latex?M%28x_i%29%20%3D%20%5Csqrt%7Ba_x%28x_i%29%5E2%20&amp;plus;%20a_y%28x_i%29%5E2%20&amp;plus;%20a_z%28x_i%29%5E2%7D)</t>
   </si>
 </sst>
 </file>
@@ -734,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99790EE8-D33A-9F4A-A9A3-8D9D28F19278}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,16 +759,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -773,13 +779,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -787,16 +793,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="68" x14ac:dyDescent="0.2">
@@ -804,16 +810,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="51" x14ac:dyDescent="0.2">
@@ -824,13 +830,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="85" x14ac:dyDescent="0.2">
@@ -841,13 +847,13 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="102" x14ac:dyDescent="0.2">
@@ -855,16 +861,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="119" x14ac:dyDescent="0.2">
@@ -872,16 +878,16 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -911,27 +917,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="170" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -942,16 +948,16 @@
     </row>
     <row r="3" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -980,50 +986,50 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="85" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F235E4-D004-E74F-A20E-01C6D25F8A1F}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="219" zoomScaleNormal="219" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="219" zoomScaleNormal="219" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1051,42 +1057,42 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1095,16 +1101,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1112,13 +1118,13 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1127,16 +1133,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
         <v>46</v>
       </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1144,63 +1150,63 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s">
         <v>64</v>
       </c>
-      <c r="I6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" t="s">
-        <v>65</v>
-      </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -1208,13 +1214,13 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1223,16 +1229,16 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1240,13 +1246,13 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1255,16 +1261,16 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1272,14 +1278,14 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
       <c r="E9">
         <v>1</v>
       </c>
@@ -1287,16 +1293,16 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1304,31 +1310,31 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1336,13 +1342,13 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1353,13 +1359,13 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1370,13 +1376,13 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1387,13 +1393,13 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1404,13 +1410,13 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1421,30 +1427,30 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1455,13 +1461,13 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1472,13 +1478,13 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -1489,13 +1495,13 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" t="s">
-        <v>63</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1506,13 +1512,13 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1523,13 +1529,13 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1540,13 +1546,13 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1557,13 +1563,13 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24">
         <v>1</v>

</xml_diff>

<commit_message>
fixed bug event detection app not working anymore documentation
</commit_message>
<xml_diff>
--- a/doc/computers.xlsx
+++ b/doc/computers.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenix/Desktop/WORKSPACES/WDK.git/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05900AC5-AE10-204A-B052-78C49035A252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37822615-00B8-EF4E-9011-262D710C0A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39080" yWindow="1960" windowWidth="30540" windowHeight="25420" activeTab="4" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
+    <workbookView xWindow="39060" yWindow="900" windowWidth="30540" windowHeight="25420" activeTab="6" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="preprocessing" sheetId="1" r:id="rId1"/>
     <sheet name="eventDetection" sheetId="2" r:id="rId2"/>
     <sheet name="segmentation" sheetId="3" r:id="rId3"/>
-    <sheet name="feature extractors" sheetId="5" r:id="rId4"/>
-    <sheet name="classification" sheetId="6" r:id="rId5"/>
-    <sheet name="utilities" sheetId="7" r:id="rId6"/>
+    <sheet name="labeling" sheetId="8" r:id="rId4"/>
+    <sheet name="feature extractors" sheetId="5" r:id="rId5"/>
+    <sheet name="classification" sheetId="6" r:id="rId6"/>
+    <sheet name="utilities" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="176">
   <si>
     <t>HighPassFilter</t>
   </si>
@@ -149,9 +150,6 @@
     <t>RMS</t>
   </si>
   <si>
-    <t>SignalVectorMagnitude</t>
-  </si>
-  <si>
     <t>Skewness</t>
   </si>
   <si>
@@ -368,9 +366,6 @@
     <t>Distribution of power into frequency components. *Note: outputs n coefficients*</t>
   </si>
   <si>
-    <t>$n^2$</t>
-  </si>
-  <si>
     <t>Memory</t>
   </si>
   <si>
@@ -386,27 +381,15 @@
     <t>TreeClassifier</t>
   </si>
   <si>
-    <t>Properties: $maxNumSplits$</t>
-  </si>
-  <si>
     <t>KNNClassifier</t>
   </si>
   <si>
     <t>EnsembleClassifier</t>
   </si>
   <si>
-    <t>Properties: $nLearners$</t>
-  </si>
-  <si>
     <t>SVMClassifier</t>
   </si>
   <si>
-    <t>Support Vector Machine. Properties: $order$, $boxConstraint$</t>
-  </si>
-  <si>
-    <t>K Nearest Neighbors classifier. Properties: $nNeighbors$, $distanceMetric$</t>
-  </si>
-  <si>
     <t>FeatureExtractor</t>
   </si>
   <si>
@@ -524,16 +507,58 @@
     <t>Invocations to time-domain feature extraction algorithms produce a single value except for the Quantile component which produces *numQuantileParts* values.</t>
   </si>
   <si>
-    <t>* The amount of memory and output size of the *PropertyGetter* and *NoOp* modules depend on their input and configuraton values and are computed at runtime.</t>
-  </si>
-  <si>
     <t>Communication</t>
   </si>
   <si>
     <t>Normalizes a features table by subtracting the *means* property and dividing by the *stds* property. If the *shouldComputeNormalizationValues* poperty is set to *true*, it computes the *means* and *stds * properties from the input table</t>
   </si>
   <si>
-    <t>The performance metrics of each classifier depends on its configuration and are calculated at runtime.</t>
+    <t>The performance metrics of each classifier depend on its configuration and are calculated at runtime.</t>
+  </si>
+  <si>
+    <t>SMV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The amount of memory and output size of the *PropertyGetter* and *NoOp* modules depend on their input and configuration values and are computed at runtime.</t>
+  </si>
+  <si>
+    <t>EventsLabeler</t>
+  </si>
+  <si>
+    <t>EventSegmentsLabeler</t>
+  </si>
+  <si>
+    <t>RangeSegmentsLabeler</t>
+  </si>
+  <si>
+    <t>LabelMapper</t>
+  </si>
+  <si>
+    <t>Maps labels to groups</t>
+  </si>
+  <si>
+    <t>Labels events as the closest event annotation under a specified *tolerance*</t>
+  </si>
+  <si>
+    <t>Labels segments generated from an event using the *EventsLabeler*</t>
+  </si>
+  <si>
+    <t>Labels segments based on range annotations. If the *shouldContainEntireSegment* is set to *true*, segments are labeled if they are fully contained in an annotation. Otherwise, segments are labeled if their middle point is contained within a range annotation</t>
+  </si>
+  <si>
+    <t>n^2</t>
+  </si>
+  <si>
+    <t>Properties: *maxNumSplits*</t>
+  </si>
+  <si>
+    <t>K Nearest Neighbors classifier. Properties: *nNeighbors*, *distanceMetric*</t>
+  </si>
+  <si>
+    <t>Properties: *nLearners*</t>
+  </si>
+  <si>
+    <t>Support Vector Machine. Properties: *order*, *boxConstraint*</t>
   </si>
 </sst>
 </file>
@@ -950,7 +975,7 @@
   <dimension ref="B1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,13 +993,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -983,10 +1008,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -997,10 +1022,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -1011,10 +1036,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -1028,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -1042,7 +1067,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -1056,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
@@ -1070,7 +1095,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1078,7 +1103,7 @@
     </row>
     <row r="10" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1094,7 +1119,7 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,13 +1133,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -1123,10 +1148,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1138,10 +1163,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -1150,7 +1175,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1188,7 @@
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,19 +1201,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="2:6" ht="85" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>19</v>
@@ -1218,7 +1243,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1227,11 +1252,70 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CD97FF-A059-4A4E-B72E-1B68161FAD55}">
+  <dimension ref="B3:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557E002C-8107-7641-99A2-BF0AF967222A}">
   <dimension ref="B2:M48"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,26 +1331,26 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F2" s="2"/>
       <c r="I2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M2" s="2"/>
     </row>
@@ -1275,7 +1359,7 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1284,13 +1368,13 @@
         <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>104</v>
-      </c>
       <c r="K3" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>11</v>
@@ -1302,7 +1386,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1314,7 +1398,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K4" s="11">
         <v>1</v>
@@ -1328,7 +1412,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -1340,7 +1424,7 @@
         <v>30</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>11</v>
@@ -1354,10 +1438,10 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1366,10 +1450,10 @@
         <v>36</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>11</v>
@@ -1377,25 +1461,25 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L7" s="11">
         <v>1</v>
@@ -1403,25 +1487,25 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L8" s="11">
         <v>1</v>
@@ -1429,25 +1513,25 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L9" s="11">
         <v>1</v>
@@ -1455,25 +1539,25 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L10" s="11">
         <v>1</v>
@@ -1484,22 +1568,22 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L11" s="11">
         <v>1</v>
@@ -1510,10 +1594,10 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1524,10 +1608,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1538,27 +1622,27 @@
         <v>21</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -1566,13 +1650,13 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1583,10 +1667,10 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1597,10 +1681,10 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1611,10 +1695,10 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1625,10 +1709,10 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1639,10 +1723,10 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1653,13 +1737,13 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -1667,24 +1751,24 @@
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1692,13 +1776,13 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1706,7 +1790,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -1724,12 +1808,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437916AE-1E40-4F43-990E-A9DE77AEB58F}">
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1743,54 +1827,54 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="23" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1798,12 +1882,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D497E10B-50B3-574F-8EC1-2744148AE1B9}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1818,75 +1902,75 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1900,13 +1984,13 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -1917,44 +2001,44 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1968,10 +2052,10 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1980,32 +2064,32 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2014,63 +2098,63 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
         <v>146</v>
       </c>
-      <c r="C14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" t="s">
-        <v>152</v>
-      </c>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentation updated preprocessing memory computation flops normalization
</commit_message>
<xml_diff>
--- a/doc/computers.xlsx
+++ b/doc/computers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenix/Desktop/WORKSPACES/WDK.git/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37822615-00B8-EF4E-9011-262D710C0A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34D5325-9DDD-3842-A7B5-0F0D494F06E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39060" yWindow="900" windowWidth="30540" windowHeight="25420" activeTab="6" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
+    <workbookView xWindow="35500" yWindow="780" windowWidth="30540" windowHeight="25420" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="preprocessing" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="181">
   <si>
     <t>HighPassFilter</t>
   </si>
@@ -48,15 +48,9 @@
     <t>SquaredMagnitude</t>
   </si>
   <si>
-    <t>![Energy](https://latex.codecogs.com/gif.latex?E%28x_i%29%20%3D%20a_x%28x_i%29%5E2%20&amp;plus;%20a_y%28x_i%29%5E2%20&amp;plus;%20a_z%28x_i%29%5E2)</t>
-  </si>
-  <si>
     <t>Norm</t>
   </si>
   <si>
-    <t>![Norm](https://latex.codecogs.com/gif.latex?N%28x_i%29%20%3D%20%5Cleft%7C%20a_x%28x_i%29%20%5Cright%7C%20&amp;plus;%20%5Cleft%7C%20a_y%28x_i%29%20%5Cright%7C%20&amp;plus;%20%5Cleft%7C%20a_z%28x_i%29%20%5Cright%7C)</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>![S1](https://latex.codecogs.com/gif.latex?S_1%28k%2Ci%2CX_i%2CT%29%20%3D%20%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%20&amp;plus;%20max%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7B2%7D)</t>
-  </si>
-  <si>
-    <t>![S2](https://latex.codecogs.com/gif.latex?S_2%28k%2Ci%2CX_i%2CT%29%20%3D%20%5Cfrac%7B%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%7D%7Bk%7D%20&amp;plus;%20%5Cfrac%7Bmax%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7Bk%7D%7D%7B2%7D)</t>
-  </si>
-  <si>
     <t>SimplePeakDetector</t>
   </si>
   <si>
@@ -261,9 +249,6 @@
     <t>Indicates the variance in the distribution of frequencies.</t>
   </si>
   <si>
-    <t>![Magnitude](https://latex.codecogs.com/gif.latex?M%28x_i%29%20%3D%20%5Csqrt%7Ba_x%28x_i%29%5E2%20&amp;plus;%20a_y%28x_i%29%5E2%20&amp;plus;%20a_z%28x_i%29%5E2%7D)</t>
-  </si>
-  <si>
     <t>Butterworth High-pass filter with order *k*</t>
   </si>
   <si>
@@ -498,9 +483,6 @@
     <t>Invocations to frequency-domain feature extraction algorithms output a single value except for the FFT and PowerSpectrum which produce *n/2* and *n* values respectively</t>
   </si>
   <si>
-    <t>Invocations to preprocessing algorithms produce *n* values.</t>
-  </si>
-  <si>
     <t>An invocation to a segmentation algorithm produces a segment (of *segmentSize* / *segmentSizeLeft* + *segmentSizeRight* values).</t>
   </si>
   <si>
@@ -559,6 +541,39 @@
   </si>
   <si>
     <t>Support Vector Machine. Properties: *order*, *boxConstraint*</t>
+  </si>
+  <si>
+    <t>ManualSegmentation</t>
+  </si>
+  <si>
+    <t>Creates segments for each annotation (converts RangeAnnotations to segments and creates segments around each EventAnnotations). This segmentation strategy cannot be used in a real application, but is useful to study the quality of the annotations</t>
+  </si>
+  <si>
+    <t>1 / n</t>
+  </si>
+  <si>
+    <t>Invocations to preprocessing algorithms produce *n* values. The memory consumption of most preprocessing algorithms is 1 if the *inPlaceComputation* property is set to true or *n* otherwise.</t>
+  </si>
+  <si>
+    <t>Derivative</t>
+  </si>
+  <si>
+    <t>First derivative: https://latex.codecogs.com/gif.latex?D%27_i%28x%29%20%3D%20%28x_i%20-%20x_%7Bi&amp;plus;1%7D%29%20/%20%5Cdelta. Second derivative: https://latex.codecogs.com/gif.latex?D%27%27_i%28x%29%20%3D%20%28x_%7Bi-1%7D%20-%20x_i%20&amp;plus;%20x_%7Bi&amp;plus;1%7D%29%20/%20%5Cdelta%5E2</t>
+  </si>
+  <si>
+    <t>![Magnitude](https://latex.codecogs.com/gif.latex?M_i%28x%2Cy%2Cz%29%20%3D%20%5Csqrt%7Bx_i%5E2%20&amp;plus;%20y_i%5E2%20&amp;plus;%20z_i%5E2%7D)</t>
+  </si>
+  <si>
+    <t>![Energy](https://latex.codecogs.com/gif.latex?E_i%28x%2Cy%2Cz%29%20%3D%20x_i%5E2%20&amp;plus;%20y_i%5E2%20&amp;plus;%20z_i%5E2)</t>
+  </si>
+  <si>
+    <t>![Norm](https://latex.codecogs.com/gif.latex?N_i%28x%2Cy%2Cz%29%20%3D%20%5Cleft%7C%20x_i%20%5Cright%7C%20&amp;plus;%20%5Cleft%7C%20y_i%20%5Cright%7C%20&amp;plus;%20%5Cleft%7C%20z_i%20%5Cright%7C)</t>
+  </si>
+  <si>
+    <t>![S2](https://latex.codecogs.com/gif.latex?S2_i%28x%29%20%3D%20%5Cfrac%7B%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%7D%7Bk%7D%20&amp;plus;%20%5Cfrac%7Bmax%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7Bk%7D%7D%7B2%7D)</t>
+  </si>
+  <si>
+    <t>![S1](https://latex.codecogs.com/gif.latex?S1_i%28x%29%20%3D%20%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%20&amp;plus;%20max%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7B2%7D)</t>
   </si>
 </sst>
 </file>
@@ -972,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99790EE8-D33A-9F4A-A9A3-8D9D28F19278}">
-  <dimension ref="B1:F10"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,13 +1008,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -1008,13 +1023,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1022,27 +1037,27 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="51" x14ac:dyDescent="0.2">
@@ -1050,65 +1065,73 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>155</v>
+    </row>
+    <row r="12" spans="2:6" ht="170" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" display="https://latex.codecogs.com/gif.latex?S_1%28k%2Ci%2CX_i%2CT%29%20%3D%20%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%20&amp;plus;%20max%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7B2%7D" xr:uid="{131BD98A-DBB0-2E46-AF42-3A8BE2E14C8A}"/>
+    <hyperlink ref="C8" r:id="rId1" display="https://latex.codecogs.com/gif.latex?S_1%28k%2Ci%2CX_i%2CT%29%20%3D%20%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%20&amp;plus;%20max%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7B2%7D" xr:uid="{131BD98A-DBB0-2E46-AF42-3A8BE2E14C8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1119,12 +1142,12 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1133,25 +1156,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="2:6" ht="170" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1160,22 +1183,22 @@
     </row>
     <row r="3" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1185,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10BBCD1-E415-E145-B533-EFE59CA1F207}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,49 +1224,63 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="2:6" ht="85" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>156</v>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1270,39 +1307,39 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1331,74 +1368,74 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F2" s="2"/>
       <c r="I2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K4" s="11">
         <v>1</v>
@@ -1409,25 +1446,25 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L5" s="11">
         <v>1</v>
@@ -1435,51 +1472,51 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="J6" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L7" s="11">
         <v>1</v>
@@ -1487,25 +1524,25 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="L8" s="11">
         <v>1</v>
@@ -1513,25 +1550,25 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="L9" s="11">
         <v>1</v>
@@ -1539,25 +1576,25 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="L10" s="11">
         <v>1</v>
@@ -1565,25 +1602,25 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="L11" s="11">
         <v>1</v>
@@ -1591,27 +1628,27 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1619,44 +1656,44 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1664,27 +1701,27 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1692,27 +1729,27 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1720,13 +1757,13 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1734,27 +1771,27 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1762,13 +1799,13 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1776,13 +1813,13 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1790,7 +1827,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -1827,54 +1864,54 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="23" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1886,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D497E10B-50B3-574F-8EC1-2744148AE1B9}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1902,143 +1939,143 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2052,10 +2089,10 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2064,32 +2101,32 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2098,63 +2135,63 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
         <v>141</v>
       </c>
-      <c r="D14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" t="s">
-        <v>146</v>
-      </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentation fixed bugs in derivative
</commit_message>
<xml_diff>
--- a/doc/computers.xlsx
+++ b/doc/computers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenix/Desktop/WORKSPACES/WDK.git/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34D5325-9DDD-3842-A7B5-0F0D494F06E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8367214A-42A0-5A4A-80DB-BCE65A60B7E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35500" yWindow="780" windowWidth="30540" windowHeight="25420" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
+    <workbookView xWindow="36000" yWindow="820" windowWidth="30540" windowHeight="25420" xr2:uid="{16D233A6-8DE0-D344-B543-6D39CACD4C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="preprocessing" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="182">
   <si>
     <t>HighPassFilter</t>
   </si>
@@ -552,15 +552,9 @@
     <t>1 / n</t>
   </si>
   <si>
-    <t>Invocations to preprocessing algorithms produce *n* values. The memory consumption of most preprocessing algorithms is 1 if the *inPlaceComputation* property is set to true or *n* otherwise.</t>
-  </si>
-  <si>
     <t>Derivative</t>
   </si>
   <si>
-    <t>First derivative: https://latex.codecogs.com/gif.latex?D%27_i%28x%29%20%3D%20%28x_i%20-%20x_%7Bi&amp;plus;1%7D%29%20/%20%5Cdelta. Second derivative: https://latex.codecogs.com/gif.latex?D%27%27_i%28x%29%20%3D%20%28x_%7Bi-1%7D%20-%20x_i%20&amp;plus;%20x_%7Bi&amp;plus;1%7D%29%20/%20%5Cdelta%5E2</t>
-  </si>
-  <si>
     <t>![Magnitude](https://latex.codecogs.com/gif.latex?M_i%28x%2Cy%2Cz%29%20%3D%20%5Csqrt%7Bx_i%5E2%20&amp;plus;%20y_i%5E2%20&amp;plus;%20z_i%5E2%7D)</t>
   </si>
   <si>
@@ -574,6 +568,15 @@
   </si>
   <si>
     <t>![S1](https://latex.codecogs.com/gif.latex?S1_i%28x%29%20%3D%20%5Cfrac%7Bmax%28x_i%20-%20x_%7Bi-1%7D%2C...%2Cx_i%20-%20x_%7Bi-k%7D%29%20&amp;plus;%20max%28x_i-x_%7Bi&amp;plus;1%7D%2C...%2Cx_i-x_%7Bi&amp;plus;k%7D%29%7D%7B2%7D)</t>
+  </si>
+  <si>
+    <t>Invocations to preprocessing algorithms produce *n* values. The memory consumption of most preprocessing algorithms is *1* if the *inPlaceComputation* property is set to *true* or *n* otherwise.</t>
+  </si>
+  <si>
+    <t>First derivative: ![Derivative](https://latex.codecogs.com/gif.latex?D%27_i%28x%29%20%3D%20%28x_i%20-%20x_%7Bi&amp;plus;1%7D%29%20/%20%5Cdelta. Second derivative: https://latex.codecogs.com/gif.latex?D%27%27_i%28x%29%20%3D%20%28x_%7Bi-1%7D%20-%20x_i%20&amp;plus;%20x_%7Bi&amp;plus;1%7D%29%20/%20%5Cdelta%5E2)</t>
+  </si>
+  <si>
+    <t>40 n</t>
   </si>
 </sst>
 </file>
@@ -990,7 +993,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1054,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>77</v>
@@ -1065,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>78</v>
@@ -1079,7 +1082,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>78</v>
@@ -1090,10 +1093,16 @@
     </row>
     <row r="7" spans="2:6" ht="153" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="102" x14ac:dyDescent="0.2">
@@ -1101,7 +1110,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>79</v>
@@ -1115,7 +1124,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>80</v>
@@ -1124,9 +1133,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="170" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" ht="204" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>